<commit_message>
Updated GRA Excel file with the share allocated to each mechanism
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\ctrl-settings\GRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ssy02/Desktop/Postdoc Projects/eps-mexico-cpl/InputData/ctrl-settings/GRA/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887CDC77-F23A-4B4D-9D83-1ABDB233AB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="2670" windowWidth="25665" windowHeight="13515" tabRatio="698"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" tabRatio="698" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <sheet name="GRA-ntnldebtinterest" sheetId="15" r:id="rId10"/>
     <sheet name="GRA-remainder" sheetId="16" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,6 +36,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,26 +46,17 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={4F81BCB5-E56D-426A-91DB-BCF0877CB817}</author>
   </authors>
   <commentList>
-    <comment ref="C15" authorId="0" shapeId="0">
+    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     It is recommended to leave this cell set to zero and to set a non-zero value in at least one other cell in this row.</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -69,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="68">
   <si>
     <t>GRA Government Revenue Accounting</t>
   </si>
@@ -267,13 +262,19 @@
   </si>
   <si>
     <t>Government revenue handling is one of the design decisions a model user should make</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +310,19 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -365,7 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -380,11 +394,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,22 +730,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="80.86328125" customWidth="1"/>
+    <col min="2" max="2" width="80.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -736,72 +755,72 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -809,7 +828,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -817,7 +836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -825,7 +844,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -833,7 +852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -841,114 +860,114 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="13"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -960,28 +979,36 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.86328125" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -989,36 +1016,71 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B15:F15)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2/C2</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="16">
+        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" s="16">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1028,28 +1090,36 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.86328125" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1057,36 +1127,71 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B16:F16)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2/C2</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3" s="16">
+        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" s="16">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1096,7 +1201,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -1106,33 +1211,33 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>
@@ -1142,7 +1247,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
@@ -1162,7 +1267,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1182,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1202,7 +1307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1222,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1242,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1262,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1282,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1302,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1322,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1342,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>52</v>
       </c>
@@ -1352,12 +1457,12 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
@@ -1377,7 +1482,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1402,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1427,7 +1532,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1452,7 +1557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1477,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1502,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1527,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1552,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1577,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1610,67 +1715,107 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.86328125" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
-      <c r="B2">
-        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B8:F8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B2" s="15">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2/C2</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B3" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3" s="16">
+        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B4" s="15">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" s="16">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B5" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="15">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1680,68 +1825,108 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.86328125" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
-        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B9:F9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>7.5</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2/C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2.5</v>
+      </c>
+      <c r="C3">
+        <v>7.5</v>
+      </c>
+      <c r="D3" s="16">
+        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>7.5</v>
+      </c>
+      <c r="D4" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>7.5</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6">
         <v>5</v>
+      </c>
+      <c r="C6">
+        <v>7.5</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
       </c>
     </row>
   </sheetData>
@@ -1750,28 +1935,36 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.86328125" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1779,36 +1972,71 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B10:F10)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2/C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="16">
+        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1818,28 +2046,36 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.86328125" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1847,36 +2083,71 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B11:F11)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2/C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="16">
+        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1886,28 +2157,36 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.86328125" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1915,36 +2194,71 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B12:F12)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2/C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="16">
+        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1954,28 +2268,36 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.86328125" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1983,36 +2305,71 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B13:F13)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2/C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="16">
+        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2022,28 +2379,36 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.86328125" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2051,36 +2416,71 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B14:F14)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="16">
+        <f>B2/C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="16">
+        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated files using CSV export script; Fixed GRA XLS file
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ssy02/Desktop/Postdoc Projects/eps-mexico-cpl/InputData/ctrl-settings/GRA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tfranc03/Developer/eps-mexico-cpl/InputData/ctrl-settings/GRA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887CDC77-F23A-4B4D-9D83-1ABDB233AB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2314E37E-2A27-A947-A3EC-3E899D1062E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" tabRatio="698" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -63,8 +63,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="66">
   <si>
     <t>GRA Government Revenue Accounting</t>
   </si>
@@ -262,12 +284,6 @@
   </si>
   <si>
     <t>Government revenue handling is one of the design decisions a model user should make</t>
-  </si>
-  <si>
-    <t>Share</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -733,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20:B24"/>
     </sheetView>
   </sheetViews>
@@ -986,12 +1002,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1001,12 +1018,8 @@
       <c r="B1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>66</v>
-      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1016,13 +1029,7 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B15:F15)</f>
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2" s="16">
-        <f>B2/C2</f>
-        <v>0.5</v>
-      </c>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1031,13 +1038,7 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3" s="16">
-        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
-        <v>0</v>
-      </c>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1046,13 +1047,7 @@
       <c r="B4">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4" s="16">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1061,13 +1056,7 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1076,13 +1065,7 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1096,13 +1079,14 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1112,12 +1096,8 @@
       <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>66</v>
-      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1127,13 +1107,7 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B16:F16)</f>
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>15</v>
-      </c>
-      <c r="D2" s="16">
-        <f>B2/C2</f>
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1142,13 +1116,7 @@
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="D3" s="16">
-        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1157,13 +1125,7 @@
       <c r="B4">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
-      <c r="D4" s="16">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1172,13 +1134,7 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>15</v>
-      </c>
-      <c r="D5" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1187,13 +1143,7 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>15</v>
-      </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1208,13 +1158,14 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="6" width="12" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1271,19 +1222,19 @@
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
+      <c r="B8" s="15">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="D8" s="15">
+        <v>10</v>
+      </c>
+      <c r="E8" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="15">
         <v>0</v>
       </c>
     </row>
@@ -1295,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1488,19 +1439,19 @@
       </c>
       <c r="B22" s="10">
         <f>IFERROR(B8/SUM($B8:$F8),1/COUNT($B8:$F8))</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C22" s="10">
         <f t="shared" ref="C22:F22" si="0">IFERROR(C8/SUM($B8:$F8),1/COUNT($B8:$F8))</f>
-        <v>0.33333333333333331</v>
+        <v>0.125</v>
       </c>
       <c r="D22" s="10">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="E22" s="10">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.125</v>
       </c>
       <c r="F22" s="10">
         <f t="shared" si="0"/>
@@ -1517,7 +1468,7 @@
       </c>
       <c r="C23" s="10">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D23" s="10">
         <f t="shared" si="1"/>
@@ -1529,7 +1480,7 @@
       </c>
       <c r="F23" s="10">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1722,12 +1673,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1737,27 +1689,16 @@
       <c r="B1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="15">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>15</v>
-      </c>
-      <c r="D2" s="16">
-        <f>B2/C2</f>
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="B2" s="15" cm="1">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B8:F8)</f>
+        <v>5</v>
+      </c>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1766,13 +1707,7 @@
       <c r="B3" s="15">
         <v>2.5</v>
       </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="D3" s="16">
-        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
-        <v>0.16666666666666666</v>
-      </c>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1781,13 +1716,7 @@
       <c r="B4" s="15">
         <v>10</v>
       </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
-      <c r="D4" s="16">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
-      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1796,13 +1725,7 @@
       <c r="B5" s="15">
         <v>2.5</v>
       </c>
-      <c r="C5">
-        <v>15</v>
-      </c>
-      <c r="D5" s="16">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1811,16 +1734,11 @@
       <c r="B6" s="15">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>15</v>
-      </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1832,12 +1750,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1847,27 +1766,16 @@
       <c r="B1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>7.5</v>
-      </c>
-      <c r="D2" s="16">
-        <f>B2/C2</f>
-        <v>0</v>
-      </c>
+      <c r="B2" cm="1">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B9:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1876,13 +1784,7 @@
       <c r="B3">
         <v>2.5</v>
       </c>
-      <c r="C3">
-        <v>7.5</v>
-      </c>
-      <c r="D3" s="16">
-        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1891,13 +1793,7 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>7.5</v>
-      </c>
-      <c r="D4" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1906,13 +1802,7 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>7.5</v>
-      </c>
-      <c r="D5" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1921,16 +1811,11 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>7.5</v>
-      </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
-      </c>
+      <c r="D6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1942,12 +1827,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1957,12 +1843,8 @@
       <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>66</v>
-      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1972,13 +1854,7 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B10:F10)</f>
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="16">
-        <f>B2/C2</f>
-        <v>0</v>
-      </c>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1987,13 +1863,7 @@
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3" s="16">
-        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
-        <v>1</v>
-      </c>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2002,13 +1872,7 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2017,13 +1881,7 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2032,13 +1890,7 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2053,12 +1905,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D6"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2068,12 +1921,8 @@
       <c r="B1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>66</v>
-      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2083,13 +1932,7 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B11:F11)</f>
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="16">
-        <f>B2/C2</f>
-        <v>0</v>
-      </c>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2098,13 +1941,7 @@
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3" s="16">
-        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
-        <v>1</v>
-      </c>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2113,13 +1950,7 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2128,13 +1959,7 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2143,13 +1968,7 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2164,12 +1983,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2179,12 +1999,8 @@
       <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>66</v>
-      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2194,13 +2010,7 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B12:F12)</f>
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="16">
-        <f>B2/C2</f>
-        <v>0</v>
-      </c>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2209,13 +2019,7 @@
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3" s="16">
-        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
-        <v>1</v>
-      </c>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2224,13 +2028,7 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2239,13 +2037,7 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2254,13 +2046,7 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2275,12 +2061,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2290,12 +2077,8 @@
       <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>66</v>
-      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2305,13 +2088,7 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B13:F13)</f>
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="16">
-        <f>B2/C2</f>
-        <v>0</v>
-      </c>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2320,13 +2097,7 @@
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3" s="16">
-        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
-        <v>1</v>
-      </c>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2335,13 +2106,7 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2350,13 +2115,7 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2365,13 +2124,7 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2386,12 +2139,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2401,12 +2155,8 @@
       <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>66</v>
-      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2416,13 +2166,7 @@
         <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B14:F14)</f>
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="16">
-        <f>B2/C2</f>
-        <v>0</v>
-      </c>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2431,13 +2175,7 @@
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3" s="16">
-        <f t="shared" ref="D3:D6" si="0">B3/C3</f>
-        <v>1</v>
-      </c>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2446,13 +2184,7 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2461,13 +2193,7 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2476,13 +2202,7 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>